<commit_message>
Changed times for predicted breakdown
</commit_message>
<xml_diff>
--- a/_templates/Predictive-Maintainance-Board/Breakdowns_List.xlsx
+++ b/_templates/Predictive-Maintainance-Board/Breakdowns_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiashaas/git/peakboard-templates/_templates/Predictive-Maintainance-Board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D6112D-0DA4-F445-953F-9E33A003839D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2F1B2C-F435-5346-A66E-08DA0CEA33A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-56580" yWindow="-940" windowWidth="28040" windowHeight="17440" xr2:uid="{C562F520-08FA-2042-9BB2-207ABB22424F}"/>
+    <workbookView xWindow="-56580" yWindow="-4040" windowWidth="32900" windowHeight="20540" xr2:uid="{C562F520-08FA-2042-9BB2-207ABB22424F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -407,7 +407,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -434,7 +434,7 @@
         <v>43795.602777777778</v>
       </c>
       <c r="C2" s="1">
-        <v>43807.884722222225</v>
+        <v>43807.875</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -445,15 +445,15 @@
         <v>43796.568749999999</v>
       </c>
       <c r="C3" s="1">
-        <v>43799.341666666667</v>
+        <v>43799.333333333336</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>43795.583333333336</v>
+        <v>43795.6</v>
       </c>
       <c r="B4" s="1">
-        <v>43796.333333333336</v>
+        <v>43796.367361111108</v>
       </c>
       <c r="C4" s="1">
         <v>43827.916666666664</v>

</xml_diff>